<commit_message>
QR Code - Attempt 1
</commit_message>
<xml_diff>
--- a/src/MasterData - HK.xlsx
+++ b/src/MasterData - HK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24519"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rhenusasia.sharepoint.com/sites/ITMasterdata/Shared Documents/Asset Management/MasterData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihand\Desktop\Work\personal\asset_track\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCC36762-3F9F-4717-94F9-53FF00845B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5733AC-0B77-4BC7-BF6B-A87413939992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8D20B851-931F-4914-8D6F-EB4B79B502DA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8D20B851-931F-4914-8D6F-EB4B79B502DA}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterData List" sheetId="4" r:id="rId1"/>
@@ -2603,7 +2603,57 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="StandartRow" xfId="2" xr:uid="{D341DF60-ACF4-4FBD-B86A-173D83B21E3C}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2695,16 +2745,6 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2719,7 +2759,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FF38E9F-15D0-48E0-AA81-4AF32283889F}" name="Table1" displayName="Table1" ref="B2:B7" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9FF38E9F-15D0-48E0-AA81-4AF32283889F}" name="Table1" displayName="Table1" ref="B2:B7" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="B2:B7" xr:uid="{F987CA63-8346-4FA7-870D-C61A71E7BF12}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{2501224F-E25E-4B89-9B71-8A0B0ECFAB13}" name="Status (Selection) - M"/>
@@ -2729,7 +2769,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7C72481B-EA5A-4C98-BAD6-1C657FFD724C}" name="Table2" displayName="Table2" ref="B10:B18" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7C72481B-EA5A-4C98-BAD6-1C657FFD724C}" name="Table2" displayName="Table2" ref="B10:B18" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="B10:B18" xr:uid="{291C4F8E-61F0-4D55-8BC9-B21694F40B50}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{30CFAA28-842F-4F17-B7DC-419B5803FAC2}" name="Category (Selection) - M"/>
@@ -2739,7 +2779,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05E70419-7852-48AB-8EAA-B13EEE6B6BCB}" name="Table3" displayName="Table3" ref="B21:B29" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{05E70419-7852-48AB-8EAA-B13EEE6B6BCB}" name="Table3" displayName="Table3" ref="B21:B29" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="B21:B29" xr:uid="{449096C6-3E5D-4488-9D42-BCA74BF2CDC2}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{3A83D490-7CD3-4FFF-80F4-648F26809EE8}" name="Manufacturer (Selection) - M"/>
@@ -2759,13 +2799,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8E60C71A-7055-4FA4-878C-C856CDFD3617}" name="Table7" displayName="Table7" ref="E2:E280" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8E60C71A-7055-4FA4-878C-C856CDFD3617}" name="Table7" displayName="Table7" ref="E2:E280" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="E2:E280" xr:uid="{2C6EE102-7032-42B1-A945-0313F8749EA6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:E280">
     <sortCondition ref="E3:E280"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{11F8CB2F-3D00-424F-B027-1D2FBDC92594}" name="City Code Text" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{11F8CB2F-3D00-424F-B027-1D2FBDC92594}" name="City Code Text" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3071,48 +3111,48 @@
   <dimension ref="B1:AE106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="V22" sqref="V22"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="H110" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="L116" sqref="L116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="118.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="118.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="7.5" customHeight="1">
       <c r="B1"/>
     </row>
-    <row r="2" spans="2:31" ht="14.45" customHeight="1">
+    <row r="2" spans="2:31" ht="14.4" customHeight="1">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
@@ -3204,7 +3244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:31" ht="14.45" customHeight="1">
+    <row r="3" spans="2:31" ht="14.4" customHeight="1">
       <c r="B3" s="13" t="s">
         <v>7</v>
       </c>
@@ -8559,7 +8599,10 @@
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="J5:J92">
-    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="W69" r:id="rId1" xr:uid="{226C9389-C11A-49BD-9F51-B1315A7FE068}"/>
@@ -8590,7 +8633,7 @@
   <pageSetup orientation="portrait" r:id="rId24"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D92CC3FB-5287-482D-B7A5-DDEFF27B6026}">
           <x14:formula1>
             <xm:f>'Drop Down List'!$G$3:$G$4</xm:f>
@@ -8635,23 +8678,23 @@
       <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" customWidth="1"/>
-    <col min="12" max="12" width="2.85546875" customWidth="1"/>
-    <col min="13" max="13" width="29.42578125" customWidth="1"/>
-    <col min="14" max="14" width="2.85546875" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="2.88671875" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" customWidth="1"/>
+    <col min="8" max="8" width="2.88671875" customWidth="1"/>
+    <col min="9" max="9" width="29.44140625" customWidth="1"/>
+    <col min="10" max="10" width="2.88671875" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" customWidth="1"/>
+    <col min="12" max="12" width="2.88671875" customWidth="1"/>
+    <col min="13" max="13" width="29.44140625" customWidth="1"/>
+    <col min="14" max="14" width="2.88671875" customWidth="1"/>
+    <col min="15" max="15" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
@@ -10157,21 +10200,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D07647D0DD85D04092550BA6E7EC2DCD" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8087d52ef72dd01ce803bd3842d0dfb5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e4345f38-d4d7-49c3-8878-12de1fec7638" xmlns:ns3="608005fa-90ea-4630-a94b-882797bb71b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b3216a3ccf05c638ad131f91b522623" ns2:_="" ns3:_="">
     <xsd:import namespace="e4345f38-d4d7-49c3-8878-12de1fec7638"/>
@@ -10336,14 +10364,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{780833D7-7AB8-4215-ACA3-46A9FEEB1237}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D383ECCE-9CB1-4AE1-AC74-D5F99340599F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e4345f38-d4d7-49c3-8878-12de1fec7638"/>
+    <ds:schemaRef ds:uri="608005fa-90ea-4630-a94b-882797bb71b5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86406536-C692-4778-9544-E75B5C6F6F90}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86406536-C692-4778-9544-E75B5C6F6F90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D383ECCE-9CB1-4AE1-AC74-D5F99340599F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{780833D7-7AB8-4215-ACA3-46A9FEEB1237}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>